<commit_message>
Journal de bord - 25.02.19 - 01.03.19
</commit_message>
<xml_diff>
--- a/Journal de bord - 18.02.19 - 22.02.19.xlsx
+++ b/Journal de bord - 18.02.19 - 22.02.19.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IMD\Journal de bord\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinis\Desktop\Journal de bord\IMD-Journal-de-bord\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609F594A-5CB1-4F11-A2B0-8E0750877862}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F85F8713-84D5-4F2B-91AE-186CCDD85893}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{6FF9F98A-377F-4DA7-9DC3-B2393DBEC313}"/>
   </bookViews>
@@ -626,17 +626,17 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -659,7 +659,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -733,7 +733,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1594,7 +1594,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="fr-FR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1783,7 +1783,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1797,7 +1797,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1871,7 +1871,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2529,7 +2529,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="fr-FR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -2694,7 +2694,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2708,7 +2708,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2782,7 +2782,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3436,7 +3436,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="fr-FR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -3598,7 +3598,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3612,7 +3612,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4400,7 +4400,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4414,7 +4414,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4488,7 +4488,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5090,7 +5090,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="fr-FR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -5249,7 +5249,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5263,7 +5263,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5337,7 +5337,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5939,7 +5939,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="fr-FR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -6110,7 +6110,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9048,7 +9048,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -9346,18 +9346,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7603D8-C251-4269-BA1D-FE4378604C07}">
   <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.31640625" customWidth="1"/>
-    <col min="8" max="8" width="24.08984375" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
-    <row r="2" spans="2:3" ht="19.25" thickTop="1" x14ac:dyDescent="0.9">
+    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:3" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B2" s="32" t="s">
         <v>19</v>
       </c>
@@ -9365,7 +9365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="30" t="s">
         <v>22</v>
       </c>
@@ -9374,7 +9374,7 @@
         <v>0.16666666666666669</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
         <v>5</v>
       </c>
@@ -9383,7 +9383,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="30" t="s">
         <v>25</v>
       </c>
@@ -9392,7 +9392,7 @@
         <v>7.6388888888888895E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
         <v>6</v>
       </c>
@@ -9401,13 +9401,13 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="34"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="30" t="s">
         <v>12</v>
       </c>
@@ -9416,7 +9416,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="30" t="s">
         <v>13</v>
       </c>
@@ -9425,7 +9425,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="30" t="s">
         <v>14</v>
       </c>
@@ -9434,7 +9434,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="30" t="s">
         <v>21</v>
       </c>
@@ -9443,7 +9443,7 @@
         <v>5.2083333333333329E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="30" t="s">
         <v>28</v>
       </c>
@@ -9452,13 +9452,13 @@
         <v>0.2048611111111111</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="34"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="30" t="s">
         <v>20</v>
       </c>
@@ -9467,7 +9467,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="30" t="s">
         <v>15</v>
       </c>
@@ -9476,7 +9476,7 @@
         <v>0.2638888888888889</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.75">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="30" t="s">
         <v>39</v>
       </c>
@@ -9485,91 +9485,91 @@
         <v>0.3263888888888889</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="35"/>
     </row>
-    <row r="18" spans="2:6" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
-    <row r="21" spans="2:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B21" s="38" t="s">
+    <row r="18" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:6" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-    </row>
-    <row r="22" spans="2:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-    </row>
-    <row r="23" spans="2:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-    </row>
-    <row r="24" spans="2:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-    </row>
-    <row r="25" spans="2:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-    </row>
-    <row r="26" spans="2:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-    </row>
-    <row r="27" spans="2:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-    </row>
-    <row r="28" spans="2:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+    </row>
+    <row r="22" spans="2:6" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+    </row>
+    <row r="23" spans="2:6" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+    </row>
+    <row r="24" spans="2:6" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+    </row>
+    <row r="25" spans="2:6" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+    </row>
+    <row r="26" spans="2:6" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+    </row>
+    <row r="27" spans="2:6" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+    </row>
+    <row r="28" spans="2:6" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9585,19 +9585,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B369663C-6641-4F8A-93C7-146E7A44F891}">
   <dimension ref="A2:H19"/>
   <sheetViews>
-    <sheetView zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.40625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.7265625" customWidth="1"/>
-    <col min="3" max="3" width="100.26953125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" customWidth="1"/>
-    <col min="9" max="9" width="17.1328125" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="100.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -9605,15 +9605,15 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30.25" thickTop="1" thickBot="1" x14ac:dyDescent="1.5">
-      <c r="B3" s="36" t="s">
+    <row r="3" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="4" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
         <v>19</v>
       </c>
@@ -9625,7 +9625,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="45" thickTop="1" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
         <v>22</v>
       </c>
@@ -9637,7 +9637,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
@@ -9645,7 +9645,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>25</v>
       </c>
@@ -9657,7 +9657,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -9668,7 +9668,7 @@
       <c r="D8" s="9"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
@@ -9676,7 +9676,7 @@
       <c r="D9" s="9"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
@@ -9684,7 +9684,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>13</v>
       </c>
@@ -9692,7 +9692,7 @@
       <c r="D11" s="11"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
@@ -9704,7 +9704,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>21</v>
       </c>
@@ -9716,7 +9716,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="73.75" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
@@ -9728,7 +9728,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>17</v>
       </c>
@@ -9736,7 +9736,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
         <v>20</v>
       </c>
@@ -9747,21 +9747,21 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="17" spans="2:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="37">
+      <c r="C17" s="38">
         <f>SUM(D5:D16)</f>
         <v>0.34027777777777779</v>
       </c>
-      <c r="D17" s="37"/>
-    </row>
-    <row r="18" spans="2:8" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="D17" s="38"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>9</v>
       </c>
@@ -9788,19 +9788,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CFE3190-40E7-4E85-BBA3-B0BF2DF1F78F}">
   <dimension ref="B2:E20"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.40625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.7265625" customWidth="1"/>
-    <col min="3" max="3" width="89.54296875" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" customWidth="1"/>
-    <col min="9" max="9" width="17.1328125" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="89.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -9808,16 +9808,16 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
-    <row r="4" spans="2:5" ht="30.25" thickTop="1" thickBot="1" x14ac:dyDescent="1.5">
-      <c r="B4" s="36" t="s">
+    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="2:5" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="5" spans="2:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20" t="s">
         <v>19</v>
       </c>
@@ -9829,7 +9829,7 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="2:5" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>22</v>
       </c>
@@ -9840,49 +9840,49 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="28"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="28"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="28"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="28"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="28"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="28"/>
     </row>
-    <row r="13" spans="2:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
@@ -9893,7 +9893,7 @@
         <v>0.18055555555555555</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>21</v>
       </c>
@@ -9904,7 +9904,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="15" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>15</v>
       </c>
@@ -9915,14 +9915,14 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="28"/>
     </row>
-    <row r="17" spans="2:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="16" t="s">
         <v>23</v>
       </c>
@@ -9933,18 +9933,18 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="18" spans="2:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="37">
+      <c r="C18" s="38">
         <f>SUM(D6:D17)</f>
         <v>0.34027777777777779</v>
       </c>
-      <c r="D18" s="37"/>
-    </row>
-    <row r="19" spans="2:4" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="D18" s="38"/>
+    </row>
+    <row r="19" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -9968,19 +9968,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE8292B0-CD36-4638-9419-DEC18F30F2BE}">
   <dimension ref="A2:E20"/>
   <sheetViews>
-    <sheetView zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.40625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.1328125" customWidth="1"/>
-    <col min="3" max="3" width="92.40625" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" customWidth="1"/>
-    <col min="9" max="9" width="17.1328125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="92.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -9988,15 +9988,15 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
-    <row r="4" spans="1:5" ht="30.25" thickTop="1" thickBot="1" x14ac:dyDescent="1.5">
-      <c r="B4" s="36" t="s">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-    </row>
-    <row r="5" spans="1:5" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+    </row>
+    <row r="5" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20" t="s">
         <v>19</v>
       </c>
@@ -10008,7 +10008,7 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>22</v>
       </c>
@@ -10019,14 +10019,14 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -10036,7 +10036,7 @@
       <c r="C8" s="23"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
@@ -10047,14 +10047,14 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>39</v>
       </c>
@@ -10065,21 +10065,21 @@
         <v>0.23611111111111113</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
@@ -10090,7 +10090,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>15</v>
       </c>
@@ -10101,25 +10101,25 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="14"/>
     </row>
-    <row r="17" spans="2:4" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="17" spans="2:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="37">
+      <c r="C17" s="38">
         <f>SUM(D6:D16)</f>
         <v>0.3611111111111111</v>
       </c>
-      <c r="D17" s="37"/>
-    </row>
-    <row r="18" spans="2:4" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="D17" s="38"/>
+    </row>
+    <row r="18" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -10143,19 +10143,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DC0D2E-DF2C-46FF-88AF-6B2EDFD4B8A9}">
   <dimension ref="A2:D20"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.40625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.1328125" customWidth="1"/>
-    <col min="3" max="3" width="88.1328125" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" customWidth="1"/>
-    <col min="9" max="9" width="17.1328125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="88.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -10163,15 +10163,15 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
-    <row r="4" spans="1:4" ht="30.25" thickTop="1" thickBot="1" x14ac:dyDescent="1.5">
-      <c r="B4" s="36" t="s">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:4" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-    </row>
-    <row r="5" spans="1:4" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20" t="s">
         <v>19</v>
       </c>
@@ -10182,21 +10182,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="22"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -10206,7 +10206,7 @@
       <c r="C8" s="23"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -10217,14 +10217,14 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
@@ -10235,14 +10235,14 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
@@ -10253,14 +10253,14 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>15</v>
       </c>
@@ -10271,7 +10271,7 @@
         <v>9.7222222222222224E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
         <v>28</v>
       </c>
@@ -10282,18 +10282,18 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="17" spans="2:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="37">
+      <c r="C17" s="38">
         <f>SUM(D6:D16)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D17" s="37"/>
-    </row>
-    <row r="18" spans="2:4" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="D17" s="38"/>
+    </row>
+    <row r="18" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -10316,19 +10316,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7470C1D8-ADAD-4649-9559-414264B70E9A}">
   <dimension ref="A2:D20"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.40625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" customWidth="1"/>
-    <col min="9" max="9" width="17.1328125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -10336,15 +10336,15 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
-    <row r="4" spans="1:4" ht="30.25" thickTop="1" thickBot="1" x14ac:dyDescent="1.5">
-      <c r="B4" s="36" t="s">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:4" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-    </row>
-    <row r="5" spans="1:4" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20" t="s">
         <v>19</v>
       </c>
@@ -10355,7 +10355,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:4" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>26</v>
       </c>
@@ -10366,7 +10366,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
@@ -10377,7 +10377,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -10391,7 +10391,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
@@ -10402,14 +10402,14 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>39</v>
       </c>
@@ -10420,7 +10420,7 @@
         <v>9.0277777777777776E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
@@ -10431,7 +10431,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
@@ -10442,7 +10442,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
@@ -10453,14 +10453,14 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="1:4" ht="45" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="16" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
         <v>28</v>
       </c>
@@ -10471,18 +10471,18 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="17" spans="2:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="37">
+      <c r="C17" s="38">
         <f>SUM(D6:D16)</f>
         <v>0.33333333333333326</v>
       </c>
-      <c r="D17" s="37"/>
-    </row>
-    <row r="18" spans="2:4" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="D17" s="38"/>
+    </row>
+    <row r="18" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>9</v>
       </c>

</xml_diff>